<commit_message>
Exercise 3 Part 1
Explored Gapminder data set, isolated certain subsets into new objects generated tables/summaries etc.
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10112"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85645230-C5B4-B243-B9A5-E1F227EE52D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E8F22D-EDEF-1F4F-8A95-C1FFCD9DFC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="480" windowWidth="12000" windowHeight="14420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="580" windowWidth="22940" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -98,10 +98,10 @@
     <t>numeric value &gt;0</t>
   </si>
   <si>
-    <t xml:space="preserve">popular pizza flavors </t>
-  </si>
-  <si>
     <t>pepperoni, cheese, sausage, supreme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">favorite popular pizza flavors </t>
   </si>
 </sst>
 </file>
@@ -145,10 +145,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,7 +430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -701,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -757,7 +756,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
@@ -768,14 +767,14 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
         <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stumbling Block - Request for Feedback
Successfully troubleshot my issue with multi-word with spaces variables, last issue is with resulttable3 not showing up as an object (error message)
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10112"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E8F22D-EDEF-1F4F-8A95-C1FFCD9DFC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CA6CD6-FADB-0240-9208-D4EA947621DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="580" windowWidth="22940" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -431,7 +431,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>